<commit_message>
Renamed headers in dummy excel file to be 'Name' and 'Wishes'
</commit_message>
<xml_diff>
--- a/target.xlsx
+++ b/target.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="283">
   <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wishing_list</t>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wishes</t>
   </si>
   <si>
     <t xml:space="preserve">Juha Korhonen</t>
@@ -883,6 +883,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -967,13 +968,13 @@
   <dimension ref="A1:C142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="65.35"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
One participant now has wish that has "old students" in the wishes
- So now one participant has legit wishes and one wish that is not directly participant name ("vanhat n-vuoden opiskelijat"). This is to help testing with the special cases of seating wishes.
</commit_message>
<xml_diff>
--- a/target.xlsx
+++ b/target.xlsx
@@ -865,7 +865,7 @@
     <t xml:space="preserve">Marja-Liisa Tamminen</t>
   </si>
   <si>
-    <t xml:space="preserve">Alina Tamminen, Johan Tamminen, Elli Tamminen, Konsta Tamminen</t>
+    <t xml:space="preserve">Alina Tamminen, Johan Tamminen, Elli Tamminen, Konsta Tamminen, vanhat n-vuoden opiskelijat</t>
   </si>
   <si>
     <t xml:space="preserve">Akseli Karhu</t>
@@ -967,11 +967,11 @@
   </sheetPr>
   <dimension ref="A1:C142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C141" activeCellId="0" sqref="C141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.12"/>

</xml_diff>